<commit_message>
sav-430: adjust tests and visibilityStatus column
</commit_message>
<xml_diff>
--- a/packages/sync-server/__tests__/importers/user/user-current-visibility-status.xlsx
+++ b/packages/sync-server/__tests__/importers/user/user-current-visibility-status.xlsx
@@ -40,13 +40,13 @@
     <t xml:space="preserve">visibilityStatus</t>
   </si>
   <si>
-    <t xml:space="preserve">users-SepidehDehghani</t>
+    <t xml:space="preserve">users-test</t>
   </si>
   <si>
-    <t xml:space="preserve">sepideh@bes.au</t>
+    <t xml:space="preserve">test@bes.au</t>
   </si>
   <si>
-    <t xml:space="preserve">Sepideh Dehghani</t>
+    <t xml:space="preserve">Test Test</t>
   </si>
   <si>
     <t xml:space="preserve">role-TestPractitioner</t>
@@ -314,8 +314,8 @@
   </sheetPr>
   <dimension ref="A1:F1004"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3017,7 +3017,7 @@
     <row r="1187" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="sepideh@bes.au"/>
+    <hyperlink ref="B2" r:id="rId1" display="test@bes.au"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>